<commit_message>
start work change validation phone number add exemple in phoneNumberExample
</commit_message>
<xml_diff>
--- a/src/main/resources/phoneNumberExample.xlsx
+++ b/src/main/resources/phoneNumberExample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\школа ректоров Сколково\skolkovo-rectors-tinder\src\main\kotlin\admin\exemples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanPC\Desktop\школа ректоров Сколоково\skolkovo-rectors-tinder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>номер телефона</t>
   </si>
+  <si>
+    <t>+00000000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,8 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -345,20 +349,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>